<commit_message>
Tablas de interés de osTicket
Archivo XLSX en el que señalo cuales son las tablas de interés de osTicket. Ya que osTikcket cuenta con una gran cantidad de tablas en su base de datos que además de datos concretos de tickets, agentes y usuarios, contienen datos HTML, CSS, diccionarios JavaScript en campos de tipo varchar y mucho más, es necesario ver detenidamente cada tabla y campo existente.
</commit_message>
<xml_diff>
--- a/datos_osticket/tablas relevantes osTicket.xlsx
+++ b/datos_osticket/tablas relevantes osTicket.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Tabla</t>
   </si>
@@ -75,6 +75,643 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> se señala a qué departamento pertenece el agente por el id de departamento</t>
+    </r>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>Almacena los distintos departamentos que existen en la organización.</t>
+  </si>
+  <si>
+    <t>*Por defecto el id_org es 0 que es la que asigna osTicket.</t>
+  </si>
+  <si>
+    <t>Se almacena el nombre completo del usuario,id de organización , fecha de creación y fecha de actualización.</t>
+  </si>
+  <si>
+    <t>Descripción de datos de relevancia</t>
+  </si>
+  <si>
+    <t>Se almacenan datos de login de un usuario registrado como nombre de usuario dentro de la aplicación, contraseña y fecha de registro.</t>
+  </si>
+  <si>
+    <t>Se almacenan los correos electronicos de cada usuario (esté o no registrado).</t>
+  </si>
+  <si>
+    <r>
+      <t>Se almacena</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el numero de telefono de este usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>user_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> apunta al usuario de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>ost_form</t>
+  </si>
+  <si>
+    <t>ost_form_entry_values</t>
+  </si>
+  <si>
+    <t>ost_form_field</t>
+  </si>
+  <si>
+    <t>ost_form_entry</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Es utilizada para señalar el tipo de registro al que pertenecen cada una de las filas de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_entry.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cada registro señala que tipo de dato y configuración tiene cada fila de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_entry_values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Contiene toda la información que pueda presentarse en los formularios (telefonos, correos, etc).</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>entry_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de registro de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es el </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y señala que tipo de dato se almacena en value. Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es un 3, en value habrá un numero telefonico, si es un 4 será una nota adjunta al usuario.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cada fila es una conexión con un objecto, por ejemplo un usuario y esta conexión se utiliza para los distintos formularios que presenta osTicket.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U", este objeto contendrá información de un usuario.
+*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es su</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U" y </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>form_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es 1, esta fila será utilizada como formulario de contactos del usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Señala si la fila de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es información de contacto de un usuario, información de un ticket, etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>user_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> apunta al usuario de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flags</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> por defecto está en 0.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">user_id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">apunta al usuario de la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> por defecto es 9.
+*Si un registro apunta a algun usuario de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, se considera a ese usuario como registrado y no como invitado.</t>
     </r>
   </si>
   <si>
@@ -126,24 +763,6 @@
     </r>
   </si>
   <si>
-    <t>°</t>
-  </si>
-  <si>
-    <t>Almacena los distintos departamentos que existen en la organización.</t>
-  </si>
-  <si>
-    <t>*Por defecto el id_org es 0 que es la que asigna osTicket.</t>
-  </si>
-  <si>
-    <t>Se almacena el nombre completo del usuario,id de organización , fecha de creación y fecha de actualización.</t>
-  </si>
-  <si>
-    <t>Descripción de datos de relevancia</t>
-  </si>
-  <si>
-    <t>Se almacenan datos de login de un usuario registrado como nombre de usuario dentro de la aplicación, contraseña y fecha de registro.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">*En la columna </t>
     </r>
@@ -192,32 +811,125 @@
     </r>
   </si>
   <si>
-    <t>Se almacenan los correos electronicos de cada usuario (esté o no registrado).</t>
-  </si>
-  <si>
-    <r>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">user_id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">apunta al usuario de la tabla </t>
+    <r>
+      <t xml:space="preserve">* Señala si el dato o fila de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ost_form_entry_values</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es una nota, un telefono u otra información espefica.</t>
+    </r>
+  </si>
+  <si>
+    <t>ost__search</t>
+  </si>
+  <si>
+    <t>Almacena distintos objetos de osticket.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U", este registro o fila será o contendrá información de un usuario.
+*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es su </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en la tabla </t>
     </r>
     <r>
       <rPr>
@@ -238,183 +950,93 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.
-*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> por defecto es 9.
-*Si un registro apunta a algun usuario de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ost_user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, se considera a ese usuario como registrado y no como invitado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>user_id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> apunta al usuario de la tabla </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ost_user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>flags</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> por defecto está en 0.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Se almacena</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> el numero de telefono de este usuario.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>user_id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> apunta al usuario de la tabla </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ost_user</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
+      <t xml:space="preserve">.
+*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es el nombre completo del usuario.
+*Si </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>object_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> es "U", </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tiene información como el telefono, correo y notas del usuario (Esto separado por espacios).</t>
     </r>
   </si>
 </sst>
@@ -558,9 +1180,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -569,6 +1188,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,10 +1496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,27 +1512,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -920,8 +1542,8 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>20</v>
+      <c r="D3" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -933,15 +1555,15 @@
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A11" si="0">A4+1</f>
+        <f t="shared" ref="A5:A9" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -950,11 +1572,11 @@
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
+      <c r="D5" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -963,13 +1585,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -978,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -993,13 +1615,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1008,38 +1630,86 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" ref="A10:A12" si="1">A9+1</f>
+        <f t="shared" ref="A10:A14" si="1">A9+1</f>
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="10"/>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="10"/>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>